<commit_message>
Updated references to include the lizard and rockfish sequences
</commit_message>
<xml_diff>
--- a/tabular/locus/ehbv-side-data.xlsx
+++ b/tabular/locus/ehbv-side-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10209"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNArt/Hepadnaviridae-GLUE/tabular/locus/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNArt/Hepadnaviridae-GLUE/tabular/locus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D5E671A-B551-A645-B3AA-1A9620FA1109}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF55828A-EEB4-7447-9D00-EB6A1DF0648C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="460" windowWidth="23380" windowHeight="10680" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5500" yWindow="460" windowWidth="30200" windowHeight="23100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="raw digs" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17328" uniqueCount="2348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17336" uniqueCount="2352">
   <si>
     <t>organism</t>
   </si>
@@ -7071,6 +7071,18 @@
   </si>
   <si>
     <t>genus</t>
+  </si>
+  <si>
+    <t>Snake endogenous hepatitis B virus 2 consensus sequence</t>
+  </si>
+  <si>
+    <t>REF_EHBV-Herpeto.2-Serpentes</t>
+  </si>
+  <si>
+    <t>EHBV-Nackedna.1-Sebastes</t>
+  </si>
+  <si>
+    <t>Sebastes endogenous nackednaviral element</t>
   </si>
 </sst>
 </file>
@@ -7759,10 +7771,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W898"/>
+  <dimension ref="A1:W897"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A853" workbookViewId="0">
-      <selection activeCell="A862" sqref="A1:W898"/>
+    <sheetView tabSelected="1" topLeftCell="A861" workbookViewId="0">
+      <selection activeCell="B885" sqref="A1:W897"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -66615,13 +66627,13 @@
     </row>
     <row r="871" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A871" s="5" t="s">
-        <v>2290</v>
+        <v>2291</v>
       </c>
       <c r="B871" s="5" t="s">
-        <v>2340</v>
+        <v>2349</v>
       </c>
       <c r="C871" s="5" t="s">
-        <v>2328</v>
+        <v>2348</v>
       </c>
       <c r="D871" s="5" t="s">
         <v>2336</v>
@@ -66630,7 +66642,7 @@
         <v>2323</v>
       </c>
       <c r="G871" s="5" t="s">
-        <v>739</v>
+        <v>471</v>
       </c>
       <c r="H871" s="5" t="s">
         <v>1211</v>
@@ -66642,37 +66654,37 @@
         <v>1256</v>
       </c>
       <c r="K871" s="5" t="s">
-        <v>1341</v>
+        <v>1302</v>
       </c>
       <c r="L871" s="5" t="s">
-        <v>1342</v>
+        <v>1303</v>
       </c>
       <c r="M871" s="5" t="s">
-        <v>437</v>
+        <v>307</v>
       </c>
       <c r="N871" s="5" t="s">
-        <v>352</v>
+        <v>308</v>
       </c>
       <c r="O871" s="5">
-        <v>96.3</v>
+        <v>99.8</v>
       </c>
       <c r="P871" s="5">
-        <v>40.984000000000002</v>
+        <v>45.378</v>
       </c>
       <c r="Q871" s="5" t="s">
-        <v>740</v>
+        <v>472</v>
       </c>
       <c r="R871" s="5" t="s">
-        <v>741</v>
+        <v>473</v>
       </c>
       <c r="S871" s="5" t="s">
-        <v>742</v>
+        <v>474</v>
       </c>
       <c r="T871" s="5">
-        <v>1033390</v>
+        <v>12480</v>
       </c>
       <c r="U871" s="5">
-        <v>1033746</v>
+        <v>12836</v>
       </c>
       <c r="V871" s="5">
         <v>357</v>
@@ -66683,12 +66695,14 @@
     </row>
     <row r="872" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A872" s="5" t="s">
-        <v>2291</v>
+        <v>2292</v>
       </c>
       <c r="B872" s="5" t="s">
-        <v>2340</v>
-      </c>
-      <c r="C872"/>
+        <v>2349</v>
+      </c>
+      <c r="C872" s="5" t="s">
+        <v>2348</v>
+      </c>
       <c r="D872" s="5" t="s">
         <v>2336</v>
       </c>
@@ -66714,16 +66728,16 @@
         <v>1303</v>
       </c>
       <c r="M872" s="5" t="s">
-        <v>307</v>
+        <v>314</v>
       </c>
       <c r="N872" s="5" t="s">
-        <v>308</v>
+        <v>315</v>
       </c>
       <c r="O872" s="5">
-        <v>99.8</v>
+        <v>132</v>
       </c>
       <c r="P872" s="5">
-        <v>45.378</v>
+        <v>48.920999999999999</v>
       </c>
       <c r="Q872" s="5" t="s">
         <v>472</v>
@@ -66732,16 +66746,16 @@
         <v>473</v>
       </c>
       <c r="S872" s="5" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="T872" s="5">
-        <v>12480</v>
+        <v>1365</v>
       </c>
       <c r="U872" s="5">
-        <v>12836</v>
+        <v>2127</v>
       </c>
       <c r="V872" s="5">
-        <v>357</v>
+        <v>763</v>
       </c>
       <c r="W872" s="5" t="s">
         <v>2317</v>
@@ -66749,12 +66763,14 @@
     </row>
     <row r="873" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A873" s="5" t="s">
-        <v>2292</v>
+        <v>2293</v>
       </c>
       <c r="B873" s="5" t="s">
-        <v>2340</v>
-      </c>
-      <c r="C873"/>
+        <v>2349</v>
+      </c>
+      <c r="C873" s="5" t="s">
+        <v>2348</v>
+      </c>
       <c r="D873" s="5" t="s">
         <v>2336</v>
       </c>
@@ -66786,10 +66802,10 @@
         <v>315</v>
       </c>
       <c r="O873" s="5">
-        <v>132</v>
+        <v>98.2</v>
       </c>
       <c r="P873" s="5">
-        <v>48.920999999999999</v>
+        <v>51.545999999999999</v>
       </c>
       <c r="Q873" s="5" t="s">
         <v>472</v>
@@ -66798,29 +66814,31 @@
         <v>473</v>
       </c>
       <c r="S873" s="5" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="T873" s="5">
-        <v>1365</v>
+        <v>108</v>
       </c>
       <c r="U873" s="5">
-        <v>2127</v>
+        <v>416</v>
       </c>
       <c r="V873" s="5">
-        <v>763</v>
+        <v>309</v>
       </c>
       <c r="W873" s="5" t="s">
-        <v>2317</v>
+        <v>2318</v>
       </c>
     </row>
     <row r="874" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A874" s="5" t="s">
-        <v>2293</v>
+        <v>2294</v>
       </c>
       <c r="B874" s="5" t="s">
-        <v>2340</v>
-      </c>
-      <c r="C874"/>
+        <v>2349</v>
+      </c>
+      <c r="C874" s="5" t="s">
+        <v>2348</v>
+      </c>
       <c r="D874" s="5" t="s">
         <v>2336</v>
       </c>
@@ -66852,10 +66870,10 @@
         <v>315</v>
       </c>
       <c r="O874" s="5">
-        <v>98.2</v>
+        <v>107</v>
       </c>
       <c r="P874" s="5">
-        <v>51.545999999999999</v>
+        <v>49.037999999999997</v>
       </c>
       <c r="Q874" s="5" t="s">
         <v>472</v>
@@ -66864,29 +66882,31 @@
         <v>473</v>
       </c>
       <c r="S874" s="5" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="T874" s="5">
-        <v>108</v>
+        <v>1548</v>
       </c>
       <c r="U874" s="5">
-        <v>416</v>
+        <v>1874</v>
       </c>
       <c r="V874" s="5">
-        <v>309</v>
+        <v>327</v>
       </c>
       <c r="W874" s="5" t="s">
-        <v>2318</v>
+        <v>2317</v>
       </c>
     </row>
     <row r="875" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A875" s="5" t="s">
-        <v>2294</v>
+        <v>2295</v>
       </c>
       <c r="B875" s="5" t="s">
-        <v>2340</v>
-      </c>
-      <c r="C875"/>
+        <v>2349</v>
+      </c>
+      <c r="C875" s="5" t="s">
+        <v>2348</v>
+      </c>
       <c r="D875" s="5" t="s">
         <v>2336</v>
       </c>
@@ -66912,16 +66932,16 @@
         <v>1303</v>
       </c>
       <c r="M875" s="5" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="N875" s="5" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="O875" s="5">
-        <v>107</v>
+        <v>72.8</v>
       </c>
       <c r="P875" s="5">
-        <v>49.037999999999997</v>
+        <v>54.545000000000002</v>
       </c>
       <c r="Q875" s="5" t="s">
         <v>472</v>
@@ -66930,16 +66950,16 @@
         <v>473</v>
       </c>
       <c r="S875" s="5" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="T875" s="5">
-        <v>1548</v>
+        <v>1</v>
       </c>
       <c r="U875" s="5">
-        <v>1874</v>
+        <v>165</v>
       </c>
       <c r="V875" s="5">
-        <v>327</v>
+        <v>165</v>
       </c>
       <c r="W875" s="5" t="s">
         <v>2317</v>
@@ -66947,12 +66967,14 @@
     </row>
     <row r="876" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A876" s="5" t="s">
-        <v>2295</v>
+        <v>2296</v>
       </c>
       <c r="B876" s="5" t="s">
-        <v>2340</v>
-      </c>
-      <c r="C876"/>
+        <v>2349</v>
+      </c>
+      <c r="C876" s="5" t="s">
+        <v>2348</v>
+      </c>
       <c r="D876" s="5" t="s">
         <v>2336</v>
       </c>
@@ -66978,16 +67000,16 @@
         <v>1303</v>
       </c>
       <c r="M876" s="5" t="s">
-        <v>307</v>
+        <v>29</v>
       </c>
       <c r="N876" s="5" t="s">
-        <v>308</v>
+        <v>19</v>
       </c>
       <c r="O876" s="5">
-        <v>72.8</v>
+        <v>135</v>
       </c>
       <c r="P876" s="5">
-        <v>54.545000000000002</v>
+        <v>43.75</v>
       </c>
       <c r="Q876" s="5" t="s">
         <v>472</v>
@@ -66999,13 +67021,13 @@
         <v>478</v>
       </c>
       <c r="T876" s="5">
-        <v>1</v>
+        <v>1254</v>
       </c>
       <c r="U876" s="5">
-        <v>165</v>
+        <v>1745</v>
       </c>
       <c r="V876" s="5">
-        <v>165</v>
+        <v>492</v>
       </c>
       <c r="W876" s="5" t="s">
         <v>2317</v>
@@ -67013,12 +67035,14 @@
     </row>
     <row r="877" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A877" s="5" t="s">
-        <v>2296</v>
-      </c>
-      <c r="B877" s="5" t="s">
-        <v>2340</v>
-      </c>
-      <c r="C877"/>
+        <v>2297</v>
+      </c>
+      <c r="B877" s="9" t="s">
+        <v>2341</v>
+      </c>
+      <c r="C877" s="9" t="s">
+        <v>2330</v>
+      </c>
       <c r="D877" s="5" t="s">
         <v>2336</v>
       </c>
@@ -67026,7 +67050,7 @@
         <v>2323</v>
       </c>
       <c r="G877" s="5" t="s">
-        <v>471</v>
+        <v>1122</v>
       </c>
       <c r="H877" s="5" t="s">
         <v>1211</v>
@@ -67038,48 +67062,48 @@
         <v>1256</v>
       </c>
       <c r="K877" s="5" t="s">
-        <v>1302</v>
+        <v>1410</v>
       </c>
       <c r="L877" s="5" t="s">
-        <v>1303</v>
+        <v>1411</v>
       </c>
       <c r="M877" s="5" t="s">
-        <v>29</v>
+        <v>307</v>
       </c>
       <c r="N877" s="5" t="s">
-        <v>19</v>
+        <v>308</v>
       </c>
       <c r="O877" s="5">
-        <v>135</v>
+        <v>251</v>
       </c>
       <c r="P877" s="5">
-        <v>43.75</v>
+        <v>42.994</v>
       </c>
       <c r="Q877" s="5" t="s">
-        <v>472</v>
+        <v>1123</v>
       </c>
       <c r="R877" s="5" t="s">
-        <v>473</v>
+        <v>1124</v>
       </c>
       <c r="S877" s="5" t="s">
-        <v>478</v>
+        <v>1125</v>
       </c>
       <c r="T877" s="5">
-        <v>1254</v>
+        <v>8478984</v>
       </c>
       <c r="U877" s="5">
-        <v>1745</v>
+        <v>8480907</v>
       </c>
       <c r="V877" s="5">
-        <v>492</v>
+        <v>1924</v>
       </c>
       <c r="W877" s="5" t="s">
-        <v>2317</v>
+        <v>2318</v>
       </c>
     </row>
     <row r="878" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A878" s="5" t="s">
-        <v>2297</v>
+        <v>2298</v>
       </c>
       <c r="B878" s="9" t="s">
         <v>2341</v>
@@ -67112,16 +67136,16 @@
         <v>1411</v>
       </c>
       <c r="M878" s="5" t="s">
-        <v>307</v>
+        <v>351</v>
       </c>
       <c r="N878" s="5" t="s">
-        <v>308</v>
+        <v>384</v>
       </c>
       <c r="O878" s="5">
-        <v>251</v>
+        <v>105</v>
       </c>
       <c r="P878" s="5">
-        <v>42.994</v>
+        <v>33.631999999999998</v>
       </c>
       <c r="Q878" s="5" t="s">
         <v>1123</v>
@@ -67130,16 +67154,16 @@
         <v>1124</v>
       </c>
       <c r="S878" s="5" t="s">
-        <v>1125</v>
+        <v>1126</v>
       </c>
       <c r="T878" s="5">
-        <v>8478984</v>
+        <v>1169578</v>
       </c>
       <c r="U878" s="5">
-        <v>8480907</v>
+        <v>1170803</v>
       </c>
       <c r="V878" s="5">
-        <v>1924</v>
+        <v>1226</v>
       </c>
       <c r="W878" s="5" t="s">
         <v>2318</v>
@@ -67147,13 +67171,13 @@
     </row>
     <row r="879" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A879" s="5" t="s">
-        <v>2298</v>
-      </c>
-      <c r="B879" s="9" t="s">
-        <v>2341</v>
-      </c>
-      <c r="C879" s="9" t="s">
-        <v>2330</v>
+        <v>2299</v>
+      </c>
+      <c r="B879" s="5" t="s">
+        <v>2340</v>
+      </c>
+      <c r="C879" s="5" t="s">
+        <v>2328</v>
       </c>
       <c r="D879" s="5" t="s">
         <v>2336</v>
@@ -67162,7 +67186,7 @@
         <v>2323</v>
       </c>
       <c r="G879" s="5" t="s">
-        <v>1122</v>
+        <v>313</v>
       </c>
       <c r="H879" s="5" t="s">
         <v>1211</v>
@@ -67174,40 +67198,40 @@
         <v>1256</v>
       </c>
       <c r="K879" s="5" t="s">
-        <v>1410</v>
+        <v>1257</v>
       </c>
       <c r="L879" s="5" t="s">
-        <v>1411</v>
+        <v>1258</v>
       </c>
       <c r="M879" s="5" t="s">
-        <v>351</v>
+        <v>314</v>
       </c>
       <c r="N879" s="5" t="s">
-        <v>384</v>
+        <v>315</v>
       </c>
       <c r="O879" s="5">
-        <v>105</v>
+        <v>220</v>
       </c>
       <c r="P879" s="5">
-        <v>33.631999999999998</v>
+        <v>76.760999999999996</v>
       </c>
       <c r="Q879" s="5" t="s">
-        <v>1123</v>
+        <v>316</v>
       </c>
       <c r="R879" s="5" t="s">
-        <v>1124</v>
+        <v>317</v>
       </c>
       <c r="S879" s="5" t="s">
-        <v>1126</v>
+        <v>318</v>
       </c>
       <c r="T879" s="5">
-        <v>1169578</v>
+        <v>33464</v>
       </c>
       <c r="U879" s="5">
-        <v>1170803</v>
+        <v>35739</v>
       </c>
       <c r="V879" s="5">
-        <v>1226</v>
+        <v>2276</v>
       </c>
       <c r="W879" s="5" t="s">
         <v>2318</v>
@@ -67215,7 +67239,7 @@
     </row>
     <row r="880" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A880" s="5" t="s">
-        <v>2299</v>
+        <v>2300</v>
       </c>
       <c r="B880" s="5" t="s">
         <v>2340</v>
@@ -67230,7 +67254,7 @@
         <v>2323</v>
       </c>
       <c r="G880" s="5" t="s">
-        <v>313</v>
+        <v>319</v>
       </c>
       <c r="H880" s="5" t="s">
         <v>1211</v>
@@ -67254,36 +67278,36 @@
         <v>315</v>
       </c>
       <c r="O880" s="5">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="P880" s="5">
         <v>76.760999999999996</v>
       </c>
       <c r="Q880" s="5" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="R880" s="5" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="S880" s="5" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="T880" s="5">
-        <v>33464</v>
+        <v>3429</v>
       </c>
       <c r="U880" s="5">
-        <v>35739</v>
+        <v>5719</v>
       </c>
       <c r="V880" s="5">
-        <v>2276</v>
+        <v>2291</v>
       </c>
       <c r="W880" s="5" t="s">
-        <v>2318</v>
+        <v>2317</v>
       </c>
     </row>
     <row r="881" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A881" s="5" t="s">
-        <v>2300</v>
+        <v>2301</v>
       </c>
       <c r="B881" s="5" t="s">
         <v>2340</v>
@@ -67322,10 +67346,10 @@
         <v>315</v>
       </c>
       <c r="O881" s="5">
-        <v>217</v>
+        <v>392</v>
       </c>
       <c r="P881" s="5">
-        <v>76.760999999999996</v>
+        <v>54.814999999999998</v>
       </c>
       <c r="Q881" s="5" t="s">
         <v>320</v>
@@ -67334,16 +67358,16 @@
         <v>321</v>
       </c>
       <c r="S881" s="5" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="T881" s="5">
-        <v>3429</v>
+        <v>2</v>
       </c>
       <c r="U881" s="5">
-        <v>5719</v>
+        <v>1138</v>
       </c>
       <c r="V881" s="5">
-        <v>2291</v>
+        <v>1137</v>
       </c>
       <c r="W881" s="5" t="s">
         <v>2317</v>
@@ -67351,7 +67375,7 @@
     </row>
     <row r="882" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A882" s="5" t="s">
-        <v>2301</v>
+        <v>2302</v>
       </c>
       <c r="B882" s="5" t="s">
         <v>2340</v>
@@ -67390,10 +67414,10 @@
         <v>315</v>
       </c>
       <c r="O882" s="5">
-        <v>392</v>
+        <v>138</v>
       </c>
       <c r="P882" s="5">
-        <v>54.814999999999998</v>
+        <v>81.25</v>
       </c>
       <c r="Q882" s="5" t="s">
         <v>320</v>
@@ -67402,16 +67426,16 @@
         <v>321</v>
       </c>
       <c r="S882" s="5" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="T882" s="5">
-        <v>2</v>
+        <v>1769</v>
       </c>
       <c r="U882" s="5">
-        <v>1138</v>
+        <v>2462</v>
       </c>
       <c r="V882" s="5">
-        <v>1137</v>
+        <v>694</v>
       </c>
       <c r="W882" s="5" t="s">
         <v>2317</v>
@@ -67419,7 +67443,7 @@
     </row>
     <row r="883" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A883" s="5" t="s">
-        <v>2302</v>
+        <v>2303</v>
       </c>
       <c r="B883" s="5" t="s">
         <v>2340</v>
@@ -67434,7 +67458,7 @@
         <v>2323</v>
       </c>
       <c r="G883" s="5" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c r="H883" s="5" t="s">
         <v>1211</v>
@@ -67458,36 +67482,36 @@
         <v>315</v>
       </c>
       <c r="O883" s="5">
-        <v>138</v>
+        <v>219</v>
       </c>
       <c r="P883" s="5">
-        <v>81.25</v>
+        <v>80.450999999999993</v>
       </c>
       <c r="Q883" s="5" t="s">
-        <v>320</v>
+        <v>326</v>
       </c>
       <c r="R883" s="5" t="s">
-        <v>321</v>
+        <v>327</v>
       </c>
       <c r="S883" s="5" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="T883" s="5">
-        <v>1769</v>
+        <v>181915</v>
       </c>
       <c r="U883" s="5">
-        <v>2462</v>
+        <v>182747</v>
       </c>
       <c r="V883" s="5">
-        <v>694</v>
+        <v>833</v>
       </c>
       <c r="W883" s="5" t="s">
-        <v>2317</v>
+        <v>2318</v>
       </c>
     </row>
     <row r="884" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A884" s="5" t="s">
-        <v>2303</v>
+        <v>2304</v>
       </c>
       <c r="B884" s="5" t="s">
         <v>2340</v>
@@ -67526,10 +67550,10 @@
         <v>315</v>
       </c>
       <c r="O884" s="5">
-        <v>219</v>
+        <v>381</v>
       </c>
       <c r="P884" s="5">
-        <v>80.450999999999993</v>
+        <v>53.713000000000001</v>
       </c>
       <c r="Q884" s="5" t="s">
         <v>326</v>
@@ -67538,16 +67562,16 @@
         <v>327</v>
       </c>
       <c r="S884" s="5" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="T884" s="5">
-        <v>181915</v>
+        <v>115615</v>
       </c>
       <c r="U884" s="5">
-        <v>182747</v>
+        <v>116787</v>
       </c>
       <c r="V884" s="5">
-        <v>833</v>
+        <v>1173</v>
       </c>
       <c r="W884" s="5" t="s">
         <v>2318</v>
@@ -67555,7 +67579,7 @@
     </row>
     <row r="885" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A885" s="5" t="s">
-        <v>2304</v>
+        <v>2305</v>
       </c>
       <c r="B885" s="5" t="s">
         <v>2340</v>
@@ -67570,7 +67594,7 @@
         <v>2323</v>
       </c>
       <c r="G885" s="5" t="s">
-        <v>325</v>
+        <v>866</v>
       </c>
       <c r="H885" s="5" t="s">
         <v>1211</v>
@@ -67585,7 +67609,7 @@
         <v>1257</v>
       </c>
       <c r="L885" s="5" t="s">
-        <v>1258</v>
+        <v>1368</v>
       </c>
       <c r="M885" s="5" t="s">
         <v>314</v>
@@ -67594,36 +67618,36 @@
         <v>315</v>
       </c>
       <c r="O885" s="5">
-        <v>381</v>
+        <v>132</v>
       </c>
       <c r="P885" s="5">
-        <v>53.713000000000001</v>
+        <v>92.308000000000007</v>
       </c>
       <c r="Q885" s="5" t="s">
-        <v>326</v>
+        <v>867</v>
       </c>
       <c r="R885" s="5" t="s">
-        <v>327</v>
+        <v>868</v>
       </c>
       <c r="S885" s="5" t="s">
-        <v>329</v>
+        <v>869</v>
       </c>
       <c r="T885" s="5">
-        <v>115615</v>
+        <v>258556</v>
       </c>
       <c r="U885" s="5">
-        <v>116787</v>
+        <v>259219</v>
       </c>
       <c r="V885" s="5">
-        <v>1173</v>
+        <v>664</v>
       </c>
       <c r="W885" s="5" t="s">
-        <v>2318</v>
+        <v>2317</v>
       </c>
     </row>
     <row r="886" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A886" s="5" t="s">
-        <v>2305</v>
+        <v>2306</v>
       </c>
       <c r="B886" s="5" t="s">
         <v>2340</v>
@@ -67638,7 +67662,7 @@
         <v>2323</v>
       </c>
       <c r="G886" s="5" t="s">
-        <v>866</v>
+        <v>870</v>
       </c>
       <c r="H886" s="5" t="s">
         <v>1211</v>
@@ -67662,36 +67686,36 @@
         <v>315</v>
       </c>
       <c r="O886" s="5">
-        <v>132</v>
+        <v>226</v>
       </c>
       <c r="P886" s="5">
-        <v>92.308000000000007</v>
+        <v>82.706999999999994</v>
       </c>
       <c r="Q886" s="5" t="s">
-        <v>867</v>
+        <v>871</v>
       </c>
       <c r="R886" s="5" t="s">
-        <v>868</v>
+        <v>872</v>
       </c>
       <c r="S886" s="5" t="s">
-        <v>869</v>
+        <v>873</v>
       </c>
       <c r="T886" s="5">
-        <v>258556</v>
+        <v>254450</v>
       </c>
       <c r="U886" s="5">
-        <v>259219</v>
+        <v>256719</v>
       </c>
       <c r="V886" s="5">
-        <v>664</v>
+        <v>2270</v>
       </c>
       <c r="W886" s="5" t="s">
-        <v>2317</v>
+        <v>2318</v>
       </c>
     </row>
     <row r="887" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A887" s="5" t="s">
-        <v>2306</v>
+        <v>2307</v>
       </c>
       <c r="B887" s="5" t="s">
         <v>2340</v>
@@ -67706,7 +67730,7 @@
         <v>2323</v>
       </c>
       <c r="G887" s="5" t="s">
-        <v>870</v>
+        <v>1127</v>
       </c>
       <c r="H887" s="5" t="s">
         <v>1211</v>
@@ -67721,7 +67745,7 @@
         <v>1257</v>
       </c>
       <c r="L887" s="5" t="s">
-        <v>1368</v>
+        <v>1412</v>
       </c>
       <c r="M887" s="5" t="s">
         <v>314</v>
@@ -67730,28 +67754,28 @@
         <v>315</v>
       </c>
       <c r="O887" s="5">
-        <v>226</v>
+        <v>97.1</v>
       </c>
       <c r="P887" s="5">
-        <v>82.706999999999994</v>
+        <v>39.645000000000003</v>
       </c>
       <c r="Q887" s="5" t="s">
-        <v>871</v>
+        <v>1128</v>
       </c>
       <c r="R887" s="5" t="s">
-        <v>872</v>
+        <v>1129</v>
       </c>
       <c r="S887" s="5" t="s">
-        <v>873</v>
+        <v>1130</v>
       </c>
       <c r="T887" s="5">
-        <v>254450</v>
+        <v>73383</v>
       </c>
       <c r="U887" s="5">
-        <v>256719</v>
+        <v>73883</v>
       </c>
       <c r="V887" s="5">
-        <v>2270</v>
+        <v>501</v>
       </c>
       <c r="W887" s="5" t="s">
         <v>2318</v>
@@ -67759,7 +67783,7 @@
     </row>
     <row r="888" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A888" s="5" t="s">
-        <v>2307</v>
+        <v>2308</v>
       </c>
       <c r="B888" s="5" t="s">
         <v>2340</v>
@@ -67798,10 +67822,10 @@
         <v>315</v>
       </c>
       <c r="O888" s="5">
-        <v>97.1</v>
+        <v>182</v>
       </c>
       <c r="P888" s="5">
-        <v>39.645000000000003</v>
+        <v>79.31</v>
       </c>
       <c r="Q888" s="5" t="s">
         <v>1128</v>
@@ -67813,13 +67837,13 @@
         <v>1130</v>
       </c>
       <c r="T888" s="5">
-        <v>73383</v>
+        <v>75018</v>
       </c>
       <c r="U888" s="5">
-        <v>73883</v>
+        <v>75614</v>
       </c>
       <c r="V888" s="5">
-        <v>501</v>
+        <v>597</v>
       </c>
       <c r="W888" s="5" t="s">
         <v>2318</v>
@@ -67827,13 +67851,13 @@
     </row>
     <row r="889" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A889" s="5" t="s">
-        <v>2308</v>
-      </c>
-      <c r="B889" s="5" t="s">
-        <v>2340</v>
-      </c>
-      <c r="C889" s="5" t="s">
-        <v>2328</v>
+        <v>2309</v>
+      </c>
+      <c r="B889" s="9" t="s">
+        <v>2344</v>
+      </c>
+      <c r="C889" s="9" t="s">
+        <v>2331</v>
       </c>
       <c r="D889" s="5" t="s">
         <v>2336</v>
@@ -67842,52 +67866,52 @@
         <v>2323</v>
       </c>
       <c r="G889" s="5" t="s">
-        <v>1127</v>
+        <v>306</v>
       </c>
       <c r="H889" s="5" t="s">
         <v>1211</v>
       </c>
       <c r="I889" s="5" t="s">
-        <v>1255</v>
+        <v>1211</v>
       </c>
       <c r="J889" s="5" t="s">
-        <v>1256</v>
+        <v>1252</v>
       </c>
       <c r="K889" s="5" t="s">
-        <v>1257</v>
+        <v>1253</v>
       </c>
       <c r="L889" s="5" t="s">
-        <v>1412</v>
+        <v>1254</v>
       </c>
       <c r="M889" s="5" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="N889" s="5" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="O889" s="5">
-        <v>182</v>
+        <v>107</v>
       </c>
       <c r="P889" s="5">
-        <v>79.31</v>
+        <v>52.631999999999998</v>
       </c>
       <c r="Q889" s="5" t="s">
-        <v>1128</v>
+        <v>309</v>
       </c>
       <c r="R889" s="5" t="s">
-        <v>1129</v>
+        <v>310</v>
       </c>
       <c r="S889" s="5" t="s">
-        <v>1130</v>
+        <v>311</v>
       </c>
       <c r="T889" s="5">
-        <v>75018</v>
+        <v>292430</v>
       </c>
       <c r="U889" s="5">
-        <v>75614</v>
+        <v>294730</v>
       </c>
       <c r="V889" s="5">
-        <v>597</v>
+        <v>2301</v>
       </c>
       <c r="W889" s="5" t="s">
         <v>2318</v>
@@ -67895,7 +67919,7 @@
     </row>
     <row r="890" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A890" s="5" t="s">
-        <v>2309</v>
+        <v>2310</v>
       </c>
       <c r="B890" s="9" t="s">
         <v>2344</v>
@@ -67928,16 +67952,16 @@
         <v>1254</v>
       </c>
       <c r="M890" s="5" t="s">
-        <v>307</v>
+        <v>18</v>
       </c>
       <c r="N890" s="5" t="s">
-        <v>308</v>
+        <v>19</v>
       </c>
       <c r="O890" s="5">
-        <v>107</v>
+        <v>141</v>
       </c>
       <c r="P890" s="5">
-        <v>52.631999999999998</v>
+        <v>48.026000000000003</v>
       </c>
       <c r="Q890" s="5" t="s">
         <v>309</v>
@@ -67946,24 +67970,24 @@
         <v>310</v>
       </c>
       <c r="S890" s="5" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="T890" s="5">
-        <v>292430</v>
+        <v>166487</v>
       </c>
       <c r="U890" s="5">
-        <v>294730</v>
+        <v>167336</v>
       </c>
       <c r="V890" s="5">
-        <v>2301</v>
+        <v>850</v>
       </c>
       <c r="W890" s="5" t="s">
-        <v>2318</v>
+        <v>2317</v>
       </c>
     </row>
     <row r="891" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A891" s="5" t="s">
-        <v>2310</v>
+        <v>2311</v>
       </c>
       <c r="B891" s="9" t="s">
         <v>2344</v>
@@ -67978,7 +68002,7 @@
         <v>2323</v>
       </c>
       <c r="G891" s="5" t="s">
-        <v>306</v>
+        <v>408</v>
       </c>
       <c r="H891" s="5" t="s">
         <v>1211</v>
@@ -67990,40 +68014,40 @@
         <v>1252</v>
       </c>
       <c r="K891" s="5" t="s">
-        <v>1253</v>
+        <v>1287</v>
       </c>
       <c r="L891" s="5" t="s">
-        <v>1254</v>
+        <v>1288</v>
       </c>
       <c r="M891" s="5" t="s">
-        <v>18</v>
+        <v>307</v>
       </c>
       <c r="N891" s="5" t="s">
-        <v>19</v>
+        <v>308</v>
       </c>
       <c r="O891" s="5">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="P891" s="5">
-        <v>48.026000000000003</v>
+        <v>44.304000000000002</v>
       </c>
       <c r="Q891" s="5" t="s">
-        <v>309</v>
+        <v>409</v>
       </c>
       <c r="R891" s="5" t="s">
-        <v>310</v>
+        <v>410</v>
       </c>
       <c r="S891" s="5" t="s">
-        <v>312</v>
+        <v>411</v>
       </c>
       <c r="T891" s="5">
-        <v>166487</v>
+        <v>36490</v>
       </c>
       <c r="U891" s="5">
-        <v>167336</v>
+        <v>38768</v>
       </c>
       <c r="V891" s="5">
-        <v>850</v>
+        <v>2279</v>
       </c>
       <c r="W891" s="5" t="s">
         <v>2317</v>
@@ -68031,13 +68055,13 @@
     </row>
     <row r="892" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A892" s="5" t="s">
-        <v>2311</v>
-      </c>
-      <c r="B892" s="9" t="s">
-        <v>2344</v>
-      </c>
-      <c r="C892" s="9" t="s">
-        <v>2331</v>
+        <v>2312</v>
+      </c>
+      <c r="B892" s="5" t="s">
+        <v>2342</v>
+      </c>
+      <c r="C892" s="5" t="s">
+        <v>2332</v>
       </c>
       <c r="D892" s="5" t="s">
         <v>2336</v>
@@ -68046,7 +68070,7 @@
         <v>2323</v>
       </c>
       <c r="G892" s="5" t="s">
-        <v>408</v>
+        <v>261</v>
       </c>
       <c r="H892" s="5" t="s">
         <v>1211</v>
@@ -68055,43 +68079,43 @@
         <v>1211</v>
       </c>
       <c r="J892" s="5" t="s">
-        <v>1252</v>
+        <v>1231</v>
       </c>
       <c r="K892" s="5" t="s">
-        <v>1287</v>
+        <v>1232</v>
       </c>
       <c r="L892" s="5" t="s">
-        <v>1288</v>
+        <v>1233</v>
       </c>
       <c r="M892" s="5" t="s">
-        <v>307</v>
+        <v>13</v>
       </c>
       <c r="N892" s="5" t="s">
-        <v>308</v>
+        <v>14</v>
       </c>
       <c r="O892" s="5">
-        <v>133</v>
+        <v>97.4</v>
       </c>
       <c r="P892" s="5">
-        <v>44.304000000000002</v>
+        <v>30.457000000000001</v>
       </c>
       <c r="Q892" s="5" t="s">
-        <v>409</v>
+        <v>262</v>
       </c>
       <c r="R892" s="5" t="s">
-        <v>410</v>
+        <v>263</v>
       </c>
       <c r="S892" s="5" t="s">
-        <v>411</v>
+        <v>264</v>
       </c>
       <c r="T892" s="5">
-        <v>36490</v>
+        <v>1905687</v>
       </c>
       <c r="U892" s="5">
-        <v>38768</v>
+        <v>1906253</v>
       </c>
       <c r="V892" s="5">
-        <v>2279</v>
+        <v>567</v>
       </c>
       <c r="W892" s="5" t="s">
         <v>2317</v>
@@ -68099,7 +68123,7 @@
     </row>
     <row r="893" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A893" s="5" t="s">
-        <v>2312</v>
+        <v>2313</v>
       </c>
       <c r="B893" s="5" t="s">
         <v>2342</v>
@@ -68114,7 +68138,7 @@
         <v>2323</v>
       </c>
       <c r="G893" s="5" t="s">
-        <v>261</v>
+        <v>272</v>
       </c>
       <c r="H893" s="5" t="s">
         <v>1211</v>
@@ -68126,10 +68150,10 @@
         <v>1231</v>
       </c>
       <c r="K893" s="5" t="s">
-        <v>1232</v>
+        <v>1236</v>
       </c>
       <c r="L893" s="5" t="s">
-        <v>1233</v>
+        <v>1237</v>
       </c>
       <c r="M893" s="5" t="s">
         <v>13</v>
@@ -68138,28 +68162,28 @@
         <v>14</v>
       </c>
       <c r="O893" s="5">
-        <v>97.4</v>
+        <v>81.599999999999994</v>
       </c>
       <c r="P893" s="5">
-        <v>30.457000000000001</v>
+        <v>38.889000000000003</v>
       </c>
       <c r="Q893" s="5" t="s">
-        <v>262</v>
+        <v>273</v>
       </c>
       <c r="R893" s="5" t="s">
-        <v>263</v>
+        <v>274</v>
       </c>
       <c r="S893" s="5" t="s">
-        <v>264</v>
+        <v>275</v>
       </c>
       <c r="T893" s="5">
-        <v>1905687</v>
+        <v>2086005</v>
       </c>
       <c r="U893" s="5">
-        <v>1906253</v>
+        <v>2086310</v>
       </c>
       <c r="V893" s="5">
-        <v>567</v>
+        <v>306</v>
       </c>
       <c r="W893" s="5" t="s">
         <v>2317</v>
@@ -68167,7 +68191,7 @@
     </row>
     <row r="894" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A894" s="5" t="s">
-        <v>2313</v>
+        <v>2314</v>
       </c>
       <c r="B894" s="5" t="s">
         <v>2342</v>
@@ -68182,7 +68206,7 @@
         <v>2323</v>
       </c>
       <c r="G894" s="5" t="s">
-        <v>272</v>
+        <v>1038</v>
       </c>
       <c r="H894" s="5" t="s">
         <v>1211</v>
@@ -68197,7 +68221,7 @@
         <v>1236</v>
       </c>
       <c r="L894" s="5" t="s">
-        <v>1237</v>
+        <v>1402</v>
       </c>
       <c r="M894" s="5" t="s">
         <v>13</v>
@@ -68206,36 +68230,36 @@
         <v>14</v>
       </c>
       <c r="O894" s="5">
-        <v>81.599999999999994</v>
+        <v>84</v>
       </c>
       <c r="P894" s="5">
         <v>38.889000000000003</v>
       </c>
       <c r="Q894" s="5" t="s">
-        <v>273</v>
+        <v>1039</v>
       </c>
       <c r="R894" s="5" t="s">
-        <v>274</v>
+        <v>1040</v>
       </c>
       <c r="S894" s="5" t="s">
-        <v>275</v>
+        <v>1041</v>
       </c>
       <c r="T894" s="5">
-        <v>2086005</v>
+        <v>351572</v>
       </c>
       <c r="U894" s="5">
-        <v>2086310</v>
+        <v>351877</v>
       </c>
       <c r="V894" s="5">
         <v>306</v>
       </c>
       <c r="W894" s="5" t="s">
-        <v>2317</v>
+        <v>2318</v>
       </c>
     </row>
     <row r="895" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A895" s="5" t="s">
-        <v>2314</v>
+        <v>2315</v>
       </c>
       <c r="B895" s="5" t="s">
         <v>2342</v>
@@ -68250,7 +68274,7 @@
         <v>2323</v>
       </c>
       <c r="G895" s="5" t="s">
-        <v>1038</v>
+        <v>334</v>
       </c>
       <c r="H895" s="5" t="s">
         <v>1211</v>
@@ -68262,10 +68286,10 @@
         <v>1231</v>
       </c>
       <c r="K895" s="5" t="s">
-        <v>1236</v>
+        <v>1262</v>
       </c>
       <c r="L895" s="5" t="s">
-        <v>1402</v>
+        <v>1263</v>
       </c>
       <c r="M895" s="5" t="s">
         <v>13</v>
@@ -68274,36 +68298,36 @@
         <v>14</v>
       </c>
       <c r="O895" s="5">
-        <v>84</v>
+        <v>68.900000000000006</v>
       </c>
       <c r="P895" s="5">
-        <v>38.889000000000003</v>
+        <v>55.101999999999997</v>
       </c>
       <c r="Q895" s="5" t="s">
-        <v>1039</v>
+        <v>335</v>
       </c>
       <c r="R895" s="5" t="s">
-        <v>1040</v>
+        <v>336</v>
       </c>
       <c r="S895" s="5" t="s">
-        <v>1041</v>
+        <v>337</v>
       </c>
       <c r="T895" s="5">
-        <v>351572</v>
+        <v>12186336</v>
       </c>
       <c r="U895" s="5">
-        <v>351877</v>
+        <v>12186515</v>
       </c>
       <c r="V895" s="5">
-        <v>306</v>
+        <v>180</v>
       </c>
       <c r="W895" s="5" t="s">
-        <v>2318</v>
+        <v>2317</v>
       </c>
     </row>
     <row r="896" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A896" s="5" t="s">
-        <v>2315</v>
+        <v>2316</v>
       </c>
       <c r="B896" s="5" t="s">
         <v>2342</v>
@@ -68318,7 +68342,7 @@
         <v>2323</v>
       </c>
       <c r="G896" s="5" t="s">
-        <v>334</v>
+        <v>857</v>
       </c>
       <c r="H896" s="5" t="s">
         <v>1211</v>
@@ -68330,10 +68354,10 @@
         <v>1231</v>
       </c>
       <c r="K896" s="5" t="s">
-        <v>1262</v>
+        <v>1363</v>
       </c>
       <c r="L896" s="5" t="s">
-        <v>1263</v>
+        <v>1364</v>
       </c>
       <c r="M896" s="5" t="s">
         <v>13</v>
@@ -68342,28 +68366,28 @@
         <v>14</v>
       </c>
       <c r="O896" s="5">
-        <v>68.900000000000006</v>
+        <v>89.7</v>
       </c>
       <c r="P896" s="5">
-        <v>55.101999999999997</v>
+        <v>31.928000000000001</v>
       </c>
       <c r="Q896" s="5" t="s">
-        <v>335</v>
+        <v>858</v>
       </c>
       <c r="R896" s="5" t="s">
-        <v>336</v>
+        <v>859</v>
       </c>
       <c r="S896" s="5" t="s">
-        <v>337</v>
+        <v>860</v>
       </c>
       <c r="T896" s="5">
-        <v>12186336</v>
+        <v>3401484</v>
       </c>
       <c r="U896" s="5">
-        <v>12186515</v>
+        <v>3402053</v>
       </c>
       <c r="V896" s="5">
-        <v>180</v>
+        <v>570</v>
       </c>
       <c r="W896" s="5" t="s">
         <v>2317</v>
@@ -68371,143 +68395,79 @@
     </row>
     <row r="897" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A897" s="5" t="s">
-        <v>2316</v>
+        <v>1417</v>
       </c>
       <c r="B897" s="5" t="s">
-        <v>2342</v>
+        <v>2350</v>
       </c>
       <c r="C897" s="5" t="s">
-        <v>2332</v>
+        <v>2351</v>
       </c>
       <c r="D897" s="5" t="s">
         <v>2336</v>
       </c>
-      <c r="E897" s="1" t="s">
-        <v>2323</v>
+      <c r="E897" s="5" t="s">
+        <v>2335</v>
       </c>
       <c r="G897" s="5" t="s">
-        <v>857</v>
+        <v>949</v>
       </c>
       <c r="H897" s="5" t="s">
-        <v>1211</v>
+        <v>1381</v>
       </c>
       <c r="I897" s="5" t="s">
         <v>1211</v>
       </c>
       <c r="J897" s="5" t="s">
-        <v>1231</v>
+        <v>1382</v>
       </c>
       <c r="K897" s="5" t="s">
-        <v>1363</v>
+        <v>1383</v>
       </c>
       <c r="L897" s="5" t="s">
-        <v>1364</v>
+        <v>1384</v>
       </c>
       <c r="M897" s="5" t="s">
-        <v>13</v>
+        <v>950</v>
       </c>
       <c r="N897" s="5" t="s">
-        <v>14</v>
+        <v>308</v>
       </c>
       <c r="O897" s="5">
-        <v>89.7</v>
+        <v>85.9</v>
       </c>
       <c r="P897" s="5">
-        <v>31.928000000000001</v>
+        <v>34.091000000000001</v>
       </c>
       <c r="Q897" s="5" t="s">
-        <v>858</v>
+        <v>951</v>
       </c>
       <c r="R897" s="5" t="s">
-        <v>859</v>
+        <v>952</v>
       </c>
       <c r="S897" s="5" t="s">
-        <v>860</v>
+        <v>953</v>
       </c>
       <c r="T897" s="5">
-        <v>3401484</v>
+        <v>2</v>
       </c>
       <c r="U897" s="5">
-        <v>3402053</v>
+        <v>526</v>
       </c>
       <c r="V897" s="5">
-        <v>570</v>
+        <v>525</v>
       </c>
       <c r="W897" s="5" t="s">
-        <v>2317</v>
-      </c>
-    </row>
-    <row r="898" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A898" s="5" t="s">
-        <v>1417</v>
-      </c>
-      <c r="B898" s="5"/>
-      <c r="C898" s="5"/>
-      <c r="D898" s="5" t="s">
-        <v>2336</v>
-      </c>
-      <c r="E898" s="5" t="s">
-        <v>2335</v>
-      </c>
-      <c r="G898" s="5" t="s">
-        <v>949</v>
-      </c>
-      <c r="H898" s="5" t="s">
-        <v>1381</v>
-      </c>
-      <c r="I898" s="5" t="s">
-        <v>1211</v>
-      </c>
-      <c r="J898" s="5" t="s">
-        <v>1382</v>
-      </c>
-      <c r="K898" s="5" t="s">
-        <v>1383</v>
-      </c>
-      <c r="L898" s="5" t="s">
-        <v>1384</v>
-      </c>
-      <c r="M898" s="5" t="s">
-        <v>950</v>
-      </c>
-      <c r="N898" s="5" t="s">
-        <v>308</v>
-      </c>
-      <c r="O898" s="5">
-        <v>85.9</v>
-      </c>
-      <c r="P898" s="5">
-        <v>34.091000000000001</v>
-      </c>
-      <c r="Q898" s="5" t="s">
-        <v>951</v>
-      </c>
-      <c r="R898" s="5" t="s">
-        <v>952</v>
-      </c>
-      <c r="S898" s="5" t="s">
-        <v>953</v>
-      </c>
-      <c r="T898" s="5">
-        <v>2</v>
-      </c>
-      <c r="U898" s="5">
-        <v>526</v>
-      </c>
-      <c r="V898" s="5">
-        <v>525</v>
-      </c>
-      <c r="W898" s="5" t="s">
         <v>2318</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:Y900">
-    <sortCondition ref="H2:H900"/>
-    <sortCondition ref="I2:I900"/>
-    <sortCondition ref="J2:J900"/>
-    <sortCondition ref="K2:K900"/>
-    <sortCondition ref="L2:L900"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:Y899">
+    <sortCondition ref="H2:H899"/>
+    <sortCondition ref="I2:I899"/>
+    <sortCondition ref="J2:J899"/>
+    <sortCondition ref="K2:K899"/>
+    <sortCondition ref="L2:L899"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -68521,10 +68481,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAD70F83-4291-DD42-8EB6-0BA9095ABCF1}">
-  <dimension ref="A3:W5"/>
+  <dimension ref="A3:W6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -68723,6 +68683,74 @@
         <v>453</v>
       </c>
       <c r="W5" s="5" t="s">
+        <v>2317</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" s="4" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>2290</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>2340</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>2328</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>2336</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>2323</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>739</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>1211</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>1255</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>1256</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>1341</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>1342</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>437</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="O6" s="5">
+        <v>96.3</v>
+      </c>
+      <c r="P6" s="5">
+        <v>40.984000000000002</v>
+      </c>
+      <c r="Q6" s="5" t="s">
+        <v>740</v>
+      </c>
+      <c r="R6" s="5" t="s">
+        <v>741</v>
+      </c>
+      <c r="S6" s="5" t="s">
+        <v>742</v>
+      </c>
+      <c r="T6" s="5">
+        <v>1033390</v>
+      </c>
+      <c r="U6" s="5">
+        <v>1033746</v>
+      </c>
+      <c r="V6" s="5">
+        <v>357</v>
+      </c>
+      <c r="W6" s="5" t="s">
         <v>2317</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Filled in missing values
</commit_message>
<xml_diff>
--- a/tabular/locus/ehbv-side-data.xlsx
+++ b/tabular/locus/ehbv-side-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/DNArt/Hepadnaviridae-GLUE/tabular/locus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC07934-EF8A-864A-9FE1-40B647871CDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EDFE12A-C852-A54B-9D14-EBC0CD2F09CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="740" yWindow="460" windowWidth="28060" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="raw digs" sheetId="1" r:id="rId1"/>
@@ -7773,8 +7773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W897"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="A1:W897"/>
+    <sheetView tabSelected="1" topLeftCell="I305" workbookViewId="0">
+      <selection activeCell="S305" sqref="S305"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -7790,7 +7790,8 @@
     <col min="13" max="13" width="29.83203125" style="4" customWidth="1"/>
     <col min="14" max="14" width="10.83203125" style="4"/>
     <col min="15" max="17" width="11" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="10.83203125" style="4"/>
+    <col min="18" max="18" width="32.33203125" style="4" customWidth="1"/>
+    <col min="19" max="19" width="41" style="4" customWidth="1"/>
     <col min="20" max="21" width="11.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="11" style="4" bestFit="1" customWidth="1"/>
     <col min="23" max="16384" width="10.83203125" style="4"/>

</xml_diff>